<commit_message>
Updated dashboard, plenty of models, and added unmodeled spreadsheets
</commit_message>
<xml_diff>
--- a/Consumer/AutoZone.xlsx
+++ b/Consumer/AutoZone.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/To Be Modeled/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C334652D-B50E-844D-A3FC-B6965A6DCC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E35431F-544C-DC4A-82FE-5BD9D3CCCBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Sheet 1'!$B$19:$AH$19</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Sheet 1'!$B$3:$AH$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1'!$B$106:$AH$106</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sheet 1'!$B$19:$AH$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sheet 1'!$B$3:$AH$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Sheet 1'!$B$106:$AH$106</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -976,18 +962,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1025,12 +999,6 @@
     <xf numFmtId="10" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1048,6 +1016,24 @@
     <xf numFmtId="9" fontId="12" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2499,13 +2485,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>2610.0500000000002</v>
-    <v>1703.3203000000001</v>
-    <v>0.67630000000000001</v>
-    <v>-9.49</v>
-    <v>-3.7790000000000002E-3</v>
-    <v>-0.05</v>
-    <v>-1.9980000000000002E-5</v>
+    <v>2750</v>
+    <v>1780.4</v>
+    <v>0.67959999999999998</v>
+    <v>-39.79</v>
+    <v>-1.6152E-2</v>
+    <v>1.38</v>
+    <v>5.6939999999999996E-4</v>
     <v>USD</v>
     <v>AutoZone, Inc. is a retailer and distributor of automotive replacement parts and accessories in the Americas. The Company's Auto Parts Stores segment is the retailer and distributor of automotive parts and accessories through the Company's, stores in the United States, Mexico, and Brazil. Each store carries an extensive product line for cars, sport utility vehicles, vans and light trucks, including new and remanufactured automotive hard parts, maintenance items, accessories, and non-automotive products. Its other segments include ALLDATA, which produces, sells and maintains diagnostic, repair and shop management software used in the automotive repair industry and E-commerce, which includes direct sales to customers through www.autozone.com for sales that are not fulfilled by local stores. The Company has approximately 6,168 stores in the United States, 703 in Mexico, and 72 in Brazil for a total store count of 6,943.</v>
     <v>69440</v>
@@ -2513,25 +2499,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>123 S Front St, MEMPHIS, TN, 38103 US</v>
-    <v>2513.87</v>
+    <v>2474.7399999999998</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45020.958333356248</v>
+    <v>45070.998972221874</v>
     <v>0</v>
-    <v>2494.9949999999999</v>
-    <v>46031965285</v>
+    <v>2421.8200000000002</v>
+    <v>44589033674</v>
     <v>AUTOZONE, INC.</v>
     <v>AUTOZONE, INC.</v>
-    <v>2502.42</v>
-    <v>20.706700000000001</v>
-    <v>2511.54</v>
-    <v>2502.0500000000002</v>
-    <v>2502</v>
+    <v>2463.41</v>
+    <v>19.9818</v>
+    <v>2463.41</v>
+    <v>2423.62</v>
+    <v>2425</v>
     <v>18397700</v>
     <v>AZO</v>
     <v>AUTOZONE, INC. (XNYS:AZO)</v>
-    <v>120747</v>
-    <v>161172</v>
+    <v>269726</v>
+    <v>135442</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -2696,9 +2682,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -3119,10 +3105,10 @@
   <dimension ref="A1:AQ118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AL24" sqref="AL24"/>
+      <selection pane="bottomRight" activeCell="AI88" sqref="AI88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3470,19 +3456,19 @@
         <v>16252230000</v>
       </c>
       <c r="AI3" s="28">
-        <v>20678000000</v>
+        <v>17494000000</v>
       </c>
       <c r="AJ3" s="28">
-        <v>21734000000</v>
+        <v>18415000000</v>
       </c>
       <c r="AK3" s="28">
-        <v>23201000000</v>
+        <v>19241000000</v>
       </c>
       <c r="AL3" s="28">
-        <v>24617000000</v>
+        <v>19904000000</v>
       </c>
       <c r="AM3" s="28">
-        <v>25905000000</v>
+        <v>20754000000</v>
       </c>
       <c r="AN3" s="18" t="s">
         <v>109</v>
@@ -3515,7 +3501,7 @@
         <v>0.21400778210116722</v>
       </c>
       <c r="F4" s="15">
-        <f t="shared" ref="F4:AP4" si="0">(F3/E3)-1</f>
+        <f t="shared" ref="F4:AM4" si="0">(F3/E3)-1</f>
         <v>0.23931623931623935</v>
       </c>
       <c r="G4" s="15">
@@ -3632,23 +3618,23 @@
       </c>
       <c r="AI4" s="16">
         <f t="shared" si="0"/>
-        <v>0.27231770655473131</v>
+        <v>7.6406130112605997E-2</v>
       </c>
       <c r="AJ4" s="16">
         <f t="shared" si="0"/>
-        <v>5.1068768739723325E-2</v>
+        <v>5.2646621698868135E-2</v>
       </c>
       <c r="AK4" s="16">
         <f t="shared" si="0"/>
-        <v>6.7497929511364685E-2</v>
+        <v>4.4854737985338122E-2</v>
       </c>
       <c r="AL4" s="16">
         <f t="shared" si="0"/>
-        <v>6.1031852075341675E-2</v>
+        <v>3.4457668520347262E-2</v>
       </c>
       <c r="AM4" s="16">
         <f t="shared" si="0"/>
-        <v>5.2321566397205199E-2</v>
+        <v>4.2704983922829509E-2</v>
       </c>
       <c r="AN4" s="17">
         <f>(AH4+AG4+AF4)/3</f>
@@ -4120,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="15">
-        <f t="shared" ref="C9:AK9" si="1">C8/C3</f>
+        <f t="shared" ref="C9:AH9" si="1">C8/C3</f>
         <v>0</v>
       </c>
       <c r="D9" s="15">
@@ -4609,7 +4595,7 @@
         <v>0.30608902783980946</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" ref="C13:AK13" si="2">C12/C3</f>
+        <f t="shared" ref="C13:AH13" si="2">C12/C3</f>
         <v>0.30244498777506112</v>
       </c>
       <c r="D13" s="15">
@@ -5082,15 +5068,15 @@
       </c>
       <c r="AO16" s="30">
         <f>AP101/AH3</f>
-        <v>2.8323476399854051</v>
+        <v>2.7435640323820176</v>
       </c>
       <c r="AP16" s="30">
         <f>AP101/AH28</f>
-        <v>18.946283132971462</v>
+        <v>18.352387333079793</v>
       </c>
       <c r="AQ16" s="31">
         <f>AP101/AH106</f>
-        <v>18.131786932829776</v>
+        <v>17.563422571948962</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -5430,7 +5416,7 @@
         <v>0.39170896785109988</v>
       </c>
       <c r="F20" s="15">
-        <f t="shared" ref="F20:AK20" si="3">(F19/E19)-1</f>
+        <f t="shared" ref="F20:AH20" si="3">(F19/E19)-1</f>
         <v>0.37446808510638308</v>
       </c>
       <c r="G20" s="15">
@@ -6396,7 +6382,7 @@
         <v>0.37282780410742489</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" ref="F29:AK29" si="4">(F28/E28)-1</f>
+        <f t="shared" ref="F29:AH29" si="4">(F28/E28)-1</f>
         <v>0.33947065592635206</v>
       </c>
       <c r="G29" s="15">
@@ -7042,7 +7028,7 @@
         <v>8.7267521850958152E-2</v>
       </c>
       <c r="D35" s="22">
-        <f t="shared" ref="D35:AK35" si="5">(D34-C34)/C34</f>
+        <f t="shared" ref="D35:AH35" si="5">(D34-C34)/C34</f>
         <v>0.10406976776017442</v>
       </c>
       <c r="E35" s="22">
@@ -11747,7 +11733,7 @@
         <v>104</v>
       </c>
       <c r="B80" s="15" t="e">
-        <f t="shared" ref="B80:AK80" si="6">B79/B3</f>
+        <f t="shared" ref="B80:AH80" si="6">B79/B3</f>
         <v>#VALUE!</v>
       </c>
       <c r="C80" s="15" t="e">
@@ -12190,10 +12176,10 @@
       <c r="AH83" s="1">
         <v>-990686000</v>
       </c>
-      <c r="AO83" s="33" t="s">
+      <c r="AO83" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="AP83" s="34"/>
+      <c r="AP83" s="63"/>
     </row>
     <row r="84" spans="1:42" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -12298,10 +12284,10 @@
       <c r="AH84" s="1">
         <v>1224692000</v>
       </c>
-      <c r="AO84" s="35" t="s">
+      <c r="AO84" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="AP84" s="36"/>
+      <c r="AP84" s="65"/>
     </row>
     <row r="85" spans="1:42" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -12739,10 +12725,10 @@
       <c r="AH88" s="1">
         <v>0</v>
       </c>
-      <c r="AO88" s="37" t="s">
+      <c r="AO88" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="AP88" s="38">
+      <c r="AP88" s="34">
         <f>AP85/(AP86+AP87)</f>
         <v>2.1264907330824177E-2</v>
       </c>
@@ -12752,7 +12738,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="15">
-        <f t="shared" ref="B89:AK89" si="7">(-1*B88)/B3</f>
+        <f t="shared" ref="B89:AH89" si="7">(-1*B88)/B3</f>
         <v>3.8558880452582996E-2</v>
       </c>
       <c r="C89" s="15">
@@ -13105,10 +13091,10 @@
       <c r="AH91" s="1">
         <v>-87577000</v>
       </c>
-      <c r="AO91" s="37" t="s">
+      <c r="AO91" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="AP91" s="38">
+      <c r="AP91" s="34">
         <f>AP89/AP90</f>
         <v>0.21093465571494963</v>
       </c>
@@ -13216,10 +13202,10 @@
       <c r="AH92" s="1">
         <v>53882000</v>
       </c>
-      <c r="AO92" s="39" t="s">
+      <c r="AO92" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="AP92" s="40">
+      <c r="AP92" s="36">
         <f>AP88*(1-AP91)</f>
         <v>1.677940142418647E-2</v>
       </c>
@@ -13327,10 +13313,10 @@
       <c r="AH93" s="1">
         <v>-614404000</v>
       </c>
-      <c r="AO93" s="35" t="s">
+      <c r="AO93" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="AP93" s="36"/>
+      <c r="AP93" s="65"/>
     </row>
     <row r="94" spans="1:42" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -13438,7 +13424,7 @@
       <c r="AO94" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="AP94" s="41">
+      <c r="AP94" s="37">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -13545,12 +13531,12 @@
       <c r="AH95" s="1">
         <v>-567182000</v>
       </c>
-      <c r="AO95" s="42" t="s">
+      <c r="AO95" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="AP95" s="43" cm="1">
+      <c r="AP95" s="39" cm="1">
         <f t="array" ref="AP95">_FV(A1,"Beta")</f>
-        <v>0.67630000000000001</v>
+        <v>0.67959999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -13659,7 +13645,7 @@
       <c r="AO96" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="AP96" s="41">
+      <c r="AP96" s="37">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -13766,12 +13752,12 @@
       <c r="AH97" s="1">
         <v>-4359991000</v>
       </c>
-      <c r="AO97" s="39" t="s">
+      <c r="AO97" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="AP97" s="40">
+      <c r="AP97" s="36">
         <f>(AP94)+((AP95)*(AP96-AP94))</f>
-        <v>7.0064715E-2</v>
+        <v>7.0206779999999996E-2</v>
       </c>
     </row>
     <row r="98" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -13877,10 +13863,10 @@
       <c r="AH98" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AO98" s="35" t="s">
+      <c r="AO98" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="AP98" s="36"/>
+      <c r="AP98" s="65"/>
     </row>
     <row r="99" spans="1:42" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -14096,12 +14082,12 @@
       <c r="AH100" s="10">
         <v>-3470497000</v>
       </c>
-      <c r="AO100" s="37" t="s">
+      <c r="AO100" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AP100" s="38">
+      <c r="AP100" s="34">
         <f>AP99/AP103</f>
-        <v>0.16802154773980388</v>
+        <v>0.17252079392739547</v>
       </c>
     </row>
     <row r="101" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14207,12 +14193,12 @@
       <c r="AH101" s="1">
         <v>506000</v>
       </c>
-      <c r="AO101" s="42" t="s">
+      <c r="AO101" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="AP101" s="44" cm="1">
+      <c r="AP101" s="40" cm="1">
         <f t="array" ref="AP101">_FV(A1,"Market cap",TRUE)</f>
-        <v>46031965285</v>
+        <v>44589033674</v>
       </c>
     </row>
     <row r="102" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14318,12 +14304,12 @@
       <c r="AH102" s="10">
         <v>-906955000</v>
       </c>
-      <c r="AO102" s="37" t="s">
+      <c r="AO102" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AP102" s="38">
+      <c r="AP102" s="34">
         <f>AP101/AP103</f>
-        <v>0.83197845226019618</v>
+        <v>0.8274792060726045</v>
       </c>
     </row>
     <row r="103" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14429,12 +14415,12 @@
       <c r="AH103" s="1">
         <v>1171335000</v>
       </c>
-      <c r="AO103" s="39" t="s">
+      <c r="AO103" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="AP103" s="45">
+      <c r="AP103" s="41">
         <f>AP99+AP101</f>
-        <v>55328314285</v>
+        <v>53885382674</v>
       </c>
     </row>
     <row r="104" spans="1:42" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -14540,10 +14526,10 @@
       <c r="AH104" s="11">
         <v>264380000</v>
       </c>
-      <c r="AO104" s="35" t="s">
+      <c r="AO104" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="AP104" s="36"/>
+      <c r="AP104" s="65"/>
     </row>
     <row r="105" spans="1:42" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -14571,7 +14557,7 @@
         <v>0.74496644295302006</v>
       </c>
       <c r="H105" s="15">
-        <f t="shared" ref="H105:AK105" si="8">(H106/G106)-1</f>
+        <f t="shared" ref="H105:AH105" si="8">(H106/G106)-1</f>
         <v>0.46153846153846145</v>
       </c>
       <c r="I105" s="15">
@@ -14689,7 +14675,7 @@
       </c>
       <c r="AP105" s="26">
         <f>(AP100*AP92)+(AP102*AP97)</f>
-        <v>6.1111634141191029E-2</v>
+        <v>6.098944623064112E-2</v>
       </c>
     </row>
     <row r="106" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14795,35 +14781,35 @@
       <c r="AH106" s="1">
         <v>2538744000</v>
       </c>
-      <c r="AI106" s="46">
+      <c r="AI106" s="42">
         <f>AH106*(1+$AP$106)</f>
-        <v>2794770149.6842027</v>
-      </c>
-      <c r="AJ106" s="46">
+        <v>2666224563.4381833</v>
+      </c>
+      <c r="AJ106" s="42">
         <f t="shared" ref="AJ106:AM106" si="9">AI106*(1+$AP$106)</f>
-        <v>3076615913.0522261</v>
-      </c>
-      <c r="AK106" s="46">
+        <v>2800106439.5154185</v>
+      </c>
+      <c r="AK106" s="42">
         <f t="shared" si="9"/>
-        <v>3386885135.2644334</v>
-      </c>
-      <c r="AL106" s="46">
+        <v>2940711063.9266672</v>
+      </c>
+      <c r="AL106" s="42">
         <f t="shared" si="9"/>
-        <v>3728444252.9243522</v>
-      </c>
-      <c r="AM106" s="46">
+        <v>3088376012.9480224</v>
+      </c>
+      <c r="AM106" s="42">
         <f t="shared" si="9"/>
-        <v>4104448775.7862139</v>
-      </c>
-      <c r="AN106" s="47" t="s">
+        <v>3243455813.9203081</v>
+      </c>
+      <c r="AN106" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="AO106" s="48" t="s">
+      <c r="AO106" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="AP106" s="49">
+      <c r="AP106" s="45">
         <f>(SUM(AI4:AM4)/5)</f>
-        <v>0.10084756465567324</v>
+        <v>5.0214028447997806E-2</v>
       </c>
     </row>
     <row r="107" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14861,151 +14847,151 @@
       <c r="AF107" s="13"/>
       <c r="AG107" s="13"/>
       <c r="AH107" s="13"/>
-      <c r="AI107" s="47"/>
-      <c r="AJ107" s="47"/>
-      <c r="AK107" s="47"/>
-      <c r="AL107" s="47"/>
-      <c r="AM107" s="50">
+      <c r="AI107" s="43"/>
+      <c r="AJ107" s="43"/>
+      <c r="AK107" s="43"/>
+      <c r="AL107" s="43"/>
+      <c r="AM107" s="46">
         <f>AM106*(1+AP107)/(AP108-AP107)</f>
-        <v>116501512469.13669</v>
-      </c>
-      <c r="AN107" s="51" t="s">
+        <v>92375475520.315933</v>
+      </c>
+      <c r="AN107" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="AO107" s="52" t="s">
+      <c r="AO107" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="AP107" s="53">
+      <c r="AP107" s="49">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:42" ht="19" x14ac:dyDescent="0.25">
-      <c r="AI108" s="50">
+      <c r="AI108" s="46">
         <f t="shared" ref="AI108:AK108" si="10">AI107+AI106</f>
-        <v>2794770149.6842027</v>
-      </c>
-      <c r="AJ108" s="50">
+        <v>2666224563.4381833</v>
+      </c>
+      <c r="AJ108" s="46">
         <f t="shared" si="10"/>
-        <v>3076615913.0522261</v>
-      </c>
-      <c r="AK108" s="50">
+        <v>2800106439.5154185</v>
+      </c>
+      <c r="AK108" s="46">
         <f t="shared" si="10"/>
-        <v>3386885135.2644334</v>
-      </c>
-      <c r="AL108" s="50">
+        <v>2940711063.9266672</v>
+      </c>
+      <c r="AL108" s="46">
         <f>AL107+AL106</f>
-        <v>3728444252.9243522</v>
-      </c>
-      <c r="AM108" s="50">
+        <v>3088376012.9480224</v>
+      </c>
+      <c r="AM108" s="46">
         <f>AM107+AM106</f>
-        <v>120605961244.9229</v>
-      </c>
-      <c r="AN108" s="51" t="s">
+        <v>95618931334.236237</v>
+      </c>
+      <c r="AN108" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="AO108" s="54" t="s">
+      <c r="AO108" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="AP108" s="55">
+      <c r="AP108" s="51">
         <f>AP105</f>
-        <v>6.1111634141191029E-2</v>
+        <v>6.098944623064112E-2</v>
       </c>
     </row>
     <row r="109" spans="1:42" ht="19" x14ac:dyDescent="0.25">
-      <c r="AI109" s="56" t="s">
+      <c r="AI109" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="AJ109" s="57"/>
+      <c r="AJ109" s="61"/>
     </row>
     <row r="110" spans="1:42" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI110" s="58" t="s">
+      <c r="AI110" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="AJ110" s="44">
+      <c r="AJ110" s="40">
         <f>NPV(AP108,AI108,AJ108,AK108,AL108,AM108)</f>
-        <v>100794647829.61165</v>
+        <v>81019225145.036743</v>
       </c>
     </row>
     <row r="111" spans="1:42" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI111" s="58" t="s">
+      <c r="AI111" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="AJ111" s="44">
+      <c r="AJ111" s="40">
         <f>AH40</f>
         <v>264380000</v>
       </c>
     </row>
     <row r="112" spans="1:42" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI112" s="58" t="s">
+      <c r="AI112" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="AJ112" s="44">
+      <c r="AJ112" s="40">
         <f>AP99</f>
         <v>9296349000</v>
       </c>
     </row>
     <row r="113" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI113" s="58" t="s">
+      <c r="AI113" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="AJ113" s="44">
+      <c r="AJ113" s="40">
         <f>AJ110+AJ111-AJ112</f>
-        <v>91762678829.611649</v>
+        <v>71987256145.036743</v>
       </c>
     </row>
     <row r="114" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI114" s="58" t="s">
+      <c r="AI114" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="AJ114" s="59" cm="1">
-        <f t="array" ref="AJ114">_FV(A1,"Shares outstanding",TRUE)</f>
-        <v>18397700</v>
+      <c r="AJ114" s="53">
+        <f>AH34*(1+(AN16*5))</f>
+        <v>13971574.129405886</v>
       </c>
     </row>
     <row r="115" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI115" s="60" t="s">
+      <c r="AI115" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="AJ115" s="61">
+      <c r="AJ115" s="55">
         <f>AJ113/AJ114</f>
-        <v>4987.7255760019807</v>
+        <v>5152.4084171393124</v>
       </c>
     </row>
     <row r="116" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI116" s="58" t="s">
+      <c r="AI116" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="AJ116" s="62" cm="1">
+      <c r="AJ116" s="56" cm="1">
         <f t="array" ref="AJ116">_FV(A1,"Price")</f>
-        <v>2502.0500000000002</v>
+        <v>2423.62</v>
       </c>
     </row>
     <row r="117" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI117" s="63" t="s">
+      <c r="AI117" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="AJ117" s="64">
+      <c r="AJ117" s="58">
         <f>AJ115/AJ116-1</f>
-        <v>0.99345559681140672</v>
+        <v>1.1259143005666368</v>
       </c>
     </row>
     <row r="118" spans="35:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="AI118" s="63" t="s">
+      <c r="AI118" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="AJ118" s="65" t="str">
+      <c r="AJ118" s="59" t="str">
         <f>IF(AJ115&gt;AJ116,"BUY","SELL")</f>
         <v>BUY</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AI109:AJ109"/>
     <mergeCell ref="AO83:AP83"/>
     <mergeCell ref="AO84:AP84"/>
     <mergeCell ref="AO93:AP93"/>
     <mergeCell ref="AO98:AP98"/>
     <mergeCell ref="AO104:AP104"/>
-    <mergeCell ref="AI109:AJ109"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="https://roic.ai/company/AZO" display="ROIC.AI | AZO" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -15075,7 +15061,7 @@
     <hyperlink ref="AG74" r:id="rId65" tooltip="https://www.sec.gov/Archives/edgar/data/866787/000155837021013446/0001558370-21-013446-index.htm" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="AH36" r:id="rId66" tooltip="https://www.sec.gov/Archives/edgar/data/866787/000155837022015239/0001558370-22-015239-index.htm" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
     <hyperlink ref="AH74" r:id="rId67" tooltip="https://www.sec.gov/Archives/edgar/data/866787/000155837022015239/0001558370-22-015239-index.htm" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="AI1" r:id="rId68" display="https://finbox.com/NYSE:WM/explorer/revenue_proj" xr:uid="{78AAC5EA-D873-8C4F-AF87-5D3E1BF7F303}"/>
+    <hyperlink ref="AI1" r:id="rId68" display="https://finbox.com/NYSE:AZO/explorer/revenue_proj" xr:uid="{78AAC5EA-D873-8C4F-AF87-5D3E1BF7F303}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId69"/>

</xml_diff>

<commit_message>
Updated dashboard and models
</commit_message>
<xml_diff>
--- a/Consumer/AutoZone.xlsx
+++ b/Consumer/AutoZone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E35431F-544C-DC4A-82FE-5BD9D3CCCBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C297A20-3673-064B-B18A-390581AE0655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2486,12 +2486,12 @@
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>2750</v>
-    <v>1780.4</v>
-    <v>0.67959999999999998</v>
-    <v>-39.79</v>
-    <v>-1.6152E-2</v>
-    <v>1.38</v>
-    <v>5.6939999999999996E-4</v>
+    <v>1959.58</v>
+    <v>0.67779999999999996</v>
+    <v>1.04</v>
+    <v>4.2279999999999998E-4</v>
+    <v>-5.43</v>
+    <v>-2.2070000000000002E-3</v>
     <v>USD</v>
     <v>AutoZone, Inc. is a retailer and distributor of automotive replacement parts and accessories in the Americas. The Company's Auto Parts Stores segment is the retailer and distributor of automotive parts and accessories through the Company's, stores in the United States, Mexico, and Brazil. Each store carries an extensive product line for cars, sport utility vehicles, vans and light trucks, including new and remanufactured automotive hard parts, maintenance items, accessories, and non-automotive products. Its other segments include ALLDATA, which produces, sells and maintains diagnostic, repair and shop management software used in the automotive repair industry and E-commerce, which includes direct sales to customers through www.autozone.com for sales that are not fulfilled by local stores. The Company has approximately 6,168 stores in the United States, 703 in Mexico, and 72 in Brazil for a total store count of 6,943.</v>
     <v>69440</v>
@@ -2499,25 +2499,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>123 S Front St, MEMPHIS, TN, 38103 US</v>
-    <v>2474.7399999999998</v>
+    <v>2471.4699999999998</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45070.998972221874</v>
+    <v>45072.958333356248</v>
     <v>0</v>
-    <v>2421.8200000000002</v>
-    <v>44589033674</v>
+    <v>2426.5700000000002</v>
+    <v>44847900000</v>
     <v>AUTOZONE, INC.</v>
     <v>AUTOZONE, INC.</v>
-    <v>2463.41</v>
-    <v>19.9818</v>
-    <v>2463.41</v>
-    <v>2423.62</v>
-    <v>2425</v>
-    <v>18397700</v>
+    <v>2461.15</v>
+    <v>19.462399999999999</v>
+    <v>2459.75</v>
+    <v>2460.79</v>
+    <v>2455.36</v>
+    <v>18225000</v>
     <v>AZO</v>
     <v>AUTOZONE, INC. (XNYS:AZO)</v>
-    <v>269726</v>
-    <v>135442</v>
+    <v>214810</v>
+    <v>146826</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -2682,9 +2682,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>Delayed 15 minutes</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -3105,10 +3105,10 @@
   <dimension ref="A1:AQ118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI88" sqref="AI88"/>
+      <selection pane="bottomRight" activeCell="AK101" sqref="AK101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5068,15 +5068,15 @@
       </c>
       <c r="AO16" s="30">
         <f>AP101/AH3</f>
-        <v>2.7435640323820176</v>
+        <v>2.7594920820096687</v>
       </c>
       <c r="AP16" s="30">
         <f>AP101/AH28</f>
-        <v>18.352387333079793</v>
+        <v>18.458934048511608</v>
       </c>
       <c r="AQ16" s="31">
         <f>AP101/AH106</f>
-        <v>17.563422571948962</v>
+        <v>17.665388869456709</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -13536,7 +13536,7 @@
       </c>
       <c r="AP95" s="39" cm="1">
         <f t="array" ref="AP95">_FV(A1,"Beta")</f>
-        <v>0.67959999999999998</v>
+        <v>0.67779999999999996</v>
       </c>
     </row>
     <row r="96" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -13757,7 +13757,7 @@
       </c>
       <c r="AP97" s="36">
         <f>(AP94)+((AP95)*(AP96-AP94))</f>
-        <v>7.0206779999999996E-2</v>
+        <v>7.0129289999999997E-2</v>
       </c>
     </row>
     <row r="98" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14087,7 +14087,7 @@
       </c>
       <c r="AP100" s="34">
         <f>AP99/AP103</f>
-        <v>0.17252079392739547</v>
+        <v>0.17169596349928135</v>
       </c>
     </row>
     <row r="101" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14198,7 +14198,7 @@
       </c>
       <c r="AP101" s="40" cm="1">
         <f t="array" ref="AP101">_FV(A1,"Market cap",TRUE)</f>
-        <v>44589033674</v>
+        <v>44847900000</v>
       </c>
     </row>
     <row r="102" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14309,7 +14309,7 @@
       </c>
       <c r="AP102" s="34">
         <f>AP101/AP103</f>
-        <v>0.8274792060726045</v>
+        <v>0.82830403650071871</v>
       </c>
     </row>
     <row r="103" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14420,7 +14420,7 @@
       </c>
       <c r="AP103" s="41">
         <f>AP99+AP101</f>
-        <v>53885382674</v>
+        <v>54144249000</v>
       </c>
     </row>
     <row r="104" spans="1:42" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -14675,7 +14675,7 @@
       </c>
       <c r="AP105" s="26">
         <f>(AP100*AP92)+(AP102*AP97)</f>
-        <v>6.098944623064112E-2</v>
+        <v>6.0969329478396395E-2</v>
       </c>
     </row>
     <row r="106" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14853,7 +14853,7 @@
       <c r="AL107" s="43"/>
       <c r="AM107" s="46">
         <f>AM106*(1+AP107)/(AP108-AP107)</f>
-        <v>92375475520.315933</v>
+        <v>92427138828.514297</v>
       </c>
       <c r="AN107" s="47" t="s">
         <v>148</v>
@@ -14884,7 +14884,7 @@
       </c>
       <c r="AM108" s="46">
         <f>AM107+AM106</f>
-        <v>95618931334.236237</v>
+        <v>95670594642.434601</v>
       </c>
       <c r="AN108" s="47" t="s">
         <v>144</v>
@@ -14894,7 +14894,7 @@
       </c>
       <c r="AP108" s="51">
         <f>AP105</f>
-        <v>6.098944623064112E-2</v>
+        <v>6.0969329478396395E-2</v>
       </c>
     </row>
     <row r="109" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14909,7 +14909,7 @@
       </c>
       <c r="AJ110" s="40">
         <f>NPV(AP108,AI108,AJ108,AK108,AL108,AM108)</f>
-        <v>81019225145.036743</v>
+        <v>81064864461.176361</v>
       </c>
     </row>
     <row r="111" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14936,7 +14936,7 @@
       </c>
       <c r="AJ113" s="40">
         <f>AJ110+AJ111-AJ112</f>
-        <v>71987256145.036743</v>
+        <v>72032895461.176361</v>
       </c>
     </row>
     <row r="114" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14954,7 +14954,7 @@
       </c>
       <c r="AJ115" s="55">
         <f>AJ113/AJ114</f>
-        <v>5152.4084171393124</v>
+        <v>5155.6750008267982</v>
       </c>
     </row>
     <row r="116" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="AJ116" s="56" cm="1">
         <f t="array" ref="AJ116">_FV(A1,"Price")</f>
-        <v>2423.62</v>
+        <v>2460.79</v>
       </c>
     </row>
     <row r="117" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14972,7 +14972,7 @@
       </c>
       <c r="AJ117" s="58">
         <f>AJ115/AJ116-1</f>
-        <v>1.1259143005666368</v>
+        <v>1.0951300195574585</v>
       </c>
     </row>
     <row r="118" spans="35:36" ht="20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New dashboard + lots of new models
</commit_message>
<xml_diff>
--- a/Consumer/AutoZone.xlsx
+++ b/Consumer/AutoZone.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A01EA88-B749-B649-8840-A58DC7DE0E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A278C0-3CB8-EE45-BB84-B798E22D7D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,1318 +1053,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="2400"/>
-              <a:t>AZO</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.9192052980132446E-2"/>
-          <c:y val="0.10406130268199233"/>
-          <c:w val="0.87445033112582782"/>
-          <c:h val="0.7582917652534813"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet 1'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Revenue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet 1'!$B$3:$AH$3</c:f>
-              <c:numCache>
-                <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>671700000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>818000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1002300000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1216800000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1508000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1808100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2242600000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2691400000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3242900000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4116400000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4482696000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4818185000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5325510000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5457123000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5637025000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5710882000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5948355000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6169804000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6522706000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6816824000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7362618000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>8072973000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8603863000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9147530000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9475313000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10187340000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10635676000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10888676000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>11221077000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>11863743000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>12631967000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>14629585000</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>16252230000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-967D-AB4F-BA46-EE5855614749}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet 1'!$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EBITDA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet 1'!$B$19:$AH$19</c:f>
-              <c:numCache>
-                <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>46600000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81600000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>118200000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>164500000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>226100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>276600000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>330500000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>390300000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>460700000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>516300000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>561990000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>418359000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>809403000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>942755000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1017023000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1011161000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1043060000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1097280000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1176898000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1360382000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1514124000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1693070000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1842119000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2001955000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2083340000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2224575000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2360163000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2406622000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2161576000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2593490000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2820834000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3357627000</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3719000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-967D-AB4F-BA46-EE5855614749}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet 1'!$A$106</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Free Cash Flow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet 1'!$B$106:$AH$106</c:f>
-              <c:numCache>
-                <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>18000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-5400000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>38500000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3600000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-44700000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-78000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-114000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-120000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-70100000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-120900000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>263303000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>289641000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>621852000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>516013000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>453509000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>364605000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>559167000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>620720000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>677506000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>651561000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>880852000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>969934000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>845927000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1000560000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>892006000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1034544000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1078538000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1016780000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1558045000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1632463000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2262372000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2896776000</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2538744000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-967D-AB4F-BA46-EE5855614749}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
-        <c:axId val="1038801839"/>
-        <c:axId val="1038470351"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1038801839"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1038470351"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1038470351"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,###,,;\(#,###,,\);\ \-\ \-" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1038801839"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.34822224539813323"/>
-          <c:y val="0.92884837671153175"/>
-          <c:w val="0.30355550920373364"/>
-          <c:h val="4.4879045291752323E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700">
-        <a:solidFill>
-          <a:schemeClr val="lt2"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>41274</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>1587500</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>15874</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A54809F-6475-EC53-DDA3-18517BD590EF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -2486,10 +1174,12 @@
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>2750</v>
-    <v>2050.21</v>
-    <v>0.67589999999999995</v>
-    <v>-20.84</v>
-    <v>-8.5459999999999998E-3</v>
+    <v>2107.66</v>
+    <v>0.65439999999999998</v>
+    <v>18.579999999999998</v>
+    <v>7.3119999999999999E-3</v>
+    <v>10.52</v>
+    <v>4.1099999999999999E-3</v>
     <v>USD</v>
     <v>AutoZone, Inc. is a retailer and distributor of automotive replacement parts and accessories in the Americas. The Company's Auto Parts Stores segment is the retailer and distributor of automotive parts and accessories through the Company's, stores in the United States, Mexico, and Brazil. Each store carries an extensive product line for cars, sport utility vehicles, vans and light trucks, including new and remanufactured automotive hard parts, maintenance items, accessories, and non-automotive products. Its other segments include ALLDATA, which produces, sells and maintains diagnostic, repair and shop management software used in the automotive repair industry and E-commerce, which includes direct sales to customers through www.autozone.com for sales that are not fulfilled by local stores. The Company has approximately 6,168 stores in the United States, 703 in Mexico, and 72 in Brazil for a total store count of 6,943.</v>
     <v>69440</v>
@@ -2497,24 +1187,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>123 S Front St, MEMPHIS, TN, 38103 US</v>
-    <v>2438.37</v>
+    <v>2566.4299999999998</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45100.774821955471</v>
+    <v>45197.988109976563</v>
     <v>0</v>
-    <v>2415.37</v>
-    <v>43897322706</v>
+    <v>2522</v>
+    <v>45704634360</v>
     <v>AUTOZONE, INC.</v>
     <v>AUTOZONE, INC.</v>
-    <v>2437.64</v>
-    <v>19.295300000000001</v>
-    <v>2438.63</v>
-    <v>2417.79</v>
-    <v>18155970</v>
+    <v>2555.9299999999998</v>
+    <v>19.337599999999998</v>
+    <v>2540.9</v>
+    <v>2559.48</v>
+    <v>2570</v>
+    <v>17857000</v>
     <v>AZO</v>
     <v>AUTOZONE, INC. (XNYS:AZO)</v>
-    <v>66592</v>
-    <v>246591</v>
+    <v>84499</v>
+    <v>139744</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -2546,6 +1237,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -2566,6 +1259,7 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -2582,7 +1276,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="42">
+    <a count="45">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -2593,13 +1287,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -2665,13 +1362,19 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
     </spb>
     <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from close</v>
+      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -2716,6 +1419,9 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -2723,6 +1429,9 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -3084,10 +1793,10 @@
   <dimension ref="A1:AQ118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AF116" sqref="AF116"/>
+      <selection pane="bottomRight" activeCell="AM97" sqref="AM97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5047,15 +3756,15 @@
       </c>
       <c r="AO16" s="30">
         <f>AP101/AH3</f>
-        <v>2.7010030442591573</v>
+        <v>2.8122069623676258</v>
       </c>
       <c r="AP16" s="30">
         <f>AP101/AH28</f>
-        <v>18.067686218000958</v>
+        <v>18.811557093254702</v>
       </c>
       <c r="AQ16" s="31">
         <f>AP101/AH106</f>
-        <v>17.290960690010493</v>
+        <v>18.002852733477656</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -13515,7 +12224,7 @@
       </c>
       <c r="AP95" s="39" cm="1">
         <f t="array" ref="AP95">_FV(A1,"Beta")</f>
-        <v>0.67589999999999995</v>
+        <v>0.65439999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -13736,7 +12445,7 @@
       </c>
       <c r="AP97" s="36">
         <f>(AP94)+((AP95)*(AP96-AP94))</f>
-        <v>7.0047495000000001E-2</v>
+        <v>6.9121920000000003E-2</v>
       </c>
     </row>
     <row r="98" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14066,7 +12775,7 @@
       </c>
       <c r="AP100" s="34">
         <f>AP99/AP103</f>
-        <v>0.17476419096205037</v>
+        <v>0.16902150529113741</v>
       </c>
     </row>
     <row r="101" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14177,7 +12886,7 @@
       </c>
       <c r="AP101" s="40" cm="1">
         <f t="array" ref="AP101">_FV(A1,"Market cap",TRUE)</f>
-        <v>43897322706</v>
+        <v>45704634360</v>
       </c>
     </row>
     <row r="102" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14288,7 +12997,7 @@
       </c>
       <c r="AP102" s="34">
         <f>AP101/AP103</f>
-        <v>0.82523580903794957</v>
+        <v>0.83097849470886265</v>
       </c>
     </row>
     <row r="103" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14399,7 +13108,7 @@
       </c>
       <c r="AP103" s="41">
         <f>AP99+AP101</f>
-        <v>53193671706</v>
+        <v>55000983360</v>
       </c>
     </row>
     <row r="104" spans="1:42" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -14654,7 +13363,7 @@
       </c>
       <c r="AP105" s="26">
         <f>(AP100*AP92)+(AP102*AP97)</f>
-        <v>6.0738139722132156E-2</v>
+        <v>6.0274908719586684E-2</v>
       </c>
     </row>
     <row r="106" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14832,7 +13541,7 @@
       <c r="AL107" s="43"/>
       <c r="AM107" s="46">
         <f>AM106*(1+AP107)/(AP108-AP107)</f>
-        <v>93025049292.352234</v>
+        <v>94246656616.359604</v>
       </c>
       <c r="AN107" s="47" t="s">
         <v>148</v>
@@ -14846,15 +13555,15 @@
     </row>
     <row r="108" spans="1:42" ht="19" x14ac:dyDescent="0.25">
       <c r="AI108" s="46">
-        <f t="shared" ref="AI108:AK108" si="10">AI107+AI106</f>
+        <f>AI107+AI106</f>
         <v>2666224563.4381833</v>
       </c>
       <c r="AJ108" s="46">
-        <f t="shared" si="10"/>
+        <f>AJ107+AJ106</f>
         <v>2800106439.5154185</v>
       </c>
       <c r="AK108" s="46">
-        <f t="shared" si="10"/>
+        <f>AK107+AK106</f>
         <v>2940711063.9266672</v>
       </c>
       <c r="AL108" s="46">
@@ -14863,7 +13572,7 @@
       </c>
       <c r="AM108" s="46">
         <f>AM107+AM106</f>
-        <v>96268505106.272537</v>
+        <v>97490112430.279907</v>
       </c>
       <c r="AN108" s="47" t="s">
         <v>144</v>
@@ -14873,7 +13582,7 @@
       </c>
       <c r="AP108" s="51">
         <f>AP105</f>
-        <v>6.0738139722132156E-2</v>
+        <v>6.0274908719586684E-2</v>
       </c>
     </row>
     <row r="109" spans="1:42" ht="19" x14ac:dyDescent="0.25">
@@ -14888,7 +13597,7 @@
       </c>
       <c r="AJ110" s="40">
         <f>NPV(AP108,AI108,AJ108,AK108,AL108,AM108)</f>
-        <v>81593059771.958755</v>
+        <v>82672240197.465561</v>
       </c>
     </row>
     <row r="111" spans="1:42" ht="20" x14ac:dyDescent="0.25">
@@ -14915,7 +13624,7 @@
       </c>
       <c r="AJ113" s="40">
         <f>AJ110+AJ111-AJ112</f>
-        <v>72561090771.958755</v>
+        <v>73640271197.465561</v>
       </c>
     </row>
     <row r="114" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14933,7 +13642,7 @@
       </c>
       <c r="AJ115" s="55">
         <f>AJ113/AJ114</f>
-        <v>5193.4799973068084</v>
+        <v>5270.7211453343207</v>
       </c>
     </row>
     <row r="116" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14942,7 +13651,7 @@
       </c>
       <c r="AJ116" s="56" cm="1">
         <f t="array" ref="AJ116">_FV(A1,"Price")</f>
-        <v>2417.79</v>
+        <v>2559.48</v>
       </c>
     </row>
     <row r="117" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -14951,7 +13660,7 @@
       </c>
       <c r="AJ117" s="58">
         <f>AJ115/AJ116-1</f>
-        <v>1.1480277432311361</v>
+        <v>1.0592937414374486</v>
       </c>
     </row>
     <row r="118" spans="35:36" ht="20" x14ac:dyDescent="0.25">
@@ -15043,6 +13752,5 @@
     <hyperlink ref="AI1" r:id="rId68" display="https://finbox.com/NYSE:AZO/explorer/revenue_proj" xr:uid="{78AAC5EA-D873-8C4F-AF87-5D3E1BF7F303}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId69"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated models and dashboard
</commit_message>
<xml_diff>
--- a/Consumer/AutoZone.xlsx
+++ b/Consumer/AutoZone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC19D400-3059-354C-93F0-A6078A3C367E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B258657B-95F5-1C4F-BD05-F5E1D551BDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1385,7 +1385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1704,7 +1704,10 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
@@ -1738,10 +1741,12 @@
       <sheetName val="Financials"/>
       <sheetName val="Healthcare"/>
       <sheetName val="Industrials"/>
-      <sheetName val="Commodities"/>
+      <sheetName val="Basic Materials"/>
       <sheetName val="US Treasury Bonds"/>
-      <sheetName val="High Growth"/>
-      <sheetName val="GARP"/>
+      <sheetName val="Fidelity"/>
+      <sheetName val="Schwab"/>
+      <sheetName val="Top Consumer Stocks"/>
+      <sheetName val="Dividend Portfolio"/>
       <sheetName val="Watchlist"/>
       <sheetName val="Small + Speculative"/>
       <sheetName val="Highest Quality"/>
@@ -1761,7 +1766,7 @@
       <sheetData sheetId="7">
         <row r="8">
           <cell r="C8">
-            <v>4.2709999999999998E-2</v>
+            <v>4.1210000000000004E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -1774,6 +1779,8 @@
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1901,11 +1908,11 @@
     <v>Powered by Refinitiv</v>
     <v>2750</v>
     <v>2277.88</v>
-    <v>0.68440000000000001</v>
-    <v>31.82</v>
-    <v>1.2192000000000001E-2</v>
-    <v>0.25</v>
-    <v>9.4629999999999994E-5</v>
+    <v>0.68459999999999999</v>
+    <v>-12.21</v>
+    <v>-4.6379999999999998E-3</v>
+    <v>32.5</v>
+    <v>1.2402E-2</v>
     <v>USD</v>
     <v>AutoZone, Inc. is a retailer and distributor of automotive replacement parts and accessories in the Americas. Its Auto Parts Stores segment is the retailer and distributor of automotive parts and accessories through the Company's, stores in the United States, Mexico, and Brazil. Each store carries an extensive product line for cars, sport utility vehicles, vans, and light trucks, including new and remanufactured automotive hard parts, maintenance items, accessories, and non-automotive products. Its other segments include ALLDATA, which produces, sells, and maintains diagnostic, repair and shop management software used in the automotive repair industry and E-commerce, which includes direct sales to customers through www.autozone.com for sales that are not fulfilled by local stores. It also provides a sales program that offers commercial credit and delivery of parts and other products. The Company has approximately 7,140 stores in the United States, Mexico, and Brazil.</v>
     <v>71400</v>
@@ -1913,25 +1920,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>123 S Front St, MEMPHIS, TN, 38103 US</v>
-    <v>2644.57</v>
+    <v>2640</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45261.996053089846</v>
+    <v>45269.00698766172</v>
     <v>0</v>
-    <v>2603</v>
-    <v>46583959062</v>
+    <v>2610.5</v>
+    <v>45402609740</v>
     <v>AUTOZONE, INC.</v>
     <v>AUTOZONE, INC.</v>
-    <v>2616.8200000000002</v>
-    <v>19.718800000000002</v>
-    <v>2609.9299999999998</v>
-    <v>2641.75</v>
-    <v>2642</v>
-    <v>17633750</v>
+    <v>2640</v>
+    <v>19.153700000000001</v>
+    <v>2632.7</v>
+    <v>2620.4899999999998</v>
+    <v>2652.99</v>
+    <v>17326000</v>
     <v>AZO</v>
     <v>AUTOZONE, INC. (XNYS:AZO)</v>
-    <v>233808</v>
-    <v>138561</v>
+    <v>110335</v>
+    <v>153834</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -15862,7 +15869,7 @@
   <dimension ref="A1:P110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15911,7 +15918,7 @@
     <row r="3" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" cm="1">
         <f t="array" ref="A3">_FV(A1,"Market cap",TRUE)</f>
-        <v>46583959062</v>
+        <v>45402609740</v>
       </c>
       <c r="B3" s="51" t="s">
         <v>200</v>
@@ -15939,7 +15946,7 @@
       </c>
       <c r="I3" s="55">
         <f>J15*(1+I7)/(I6-I7)</f>
-        <v>73853570592.710724</v>
+        <v>74504868355.844925</v>
       </c>
       <c r="J3" s="56" t="s">
         <v>204</v>
@@ -15982,21 +15989,21 @@
       </c>
       <c r="G4" s="62">
         <f>A5*(1+(5*G3))</f>
-        <v>12611438.474594535</v>
+        <v>12391339.505824056</v>
       </c>
       <c r="H4" s="61" t="s">
         <v>210</v>
       </c>
       <c r="I4" s="39">
         <f>NPV(I6,F15,G15,H15,I15,(J15+I3))</f>
-        <v>64628498691.349091</v>
+        <v>65203430901.571449</v>
       </c>
       <c r="J4" s="61" t="s">
         <v>211</v>
       </c>
       <c r="K4" s="63" cm="1">
         <f t="array" ref="K4">_FV(A1,"Change (%)",TRUE)</f>
-        <v>1.2192000000000001E-2</v>
+        <v>-4.6379999999999998E-3</v>
       </c>
       <c r="L4" s="64" t="s">
         <v>212</v>
@@ -16011,7 +16018,7 @@
     <row r="5" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" cm="1">
         <f t="array" ref="A5">_FV(A1,"Shares outstanding",TRUE)</f>
-        <v>17633750</v>
+        <v>17326000</v>
       </c>
       <c r="B5" s="60" t="s">
         <v>214</v>
@@ -16039,14 +16046,14 @@
       </c>
       <c r="I5" s="39">
         <f>I4+G5-G6</f>
-        <v>61988506691.349091</v>
+        <v>62563438901.571449</v>
       </c>
       <c r="J5" s="61" t="s">
         <v>218</v>
       </c>
       <c r="K5" s="66" cm="1">
         <f t="array" ref="K5">_FV(A1,"Price")</f>
-        <v>2641.75</v>
+        <v>2620.4899999999998</v>
       </c>
       <c r="L5" s="67" t="s">
         <v>219</v>
@@ -16064,7 +16071,7 @@
     <row r="6" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="68">
         <f>O20/F10</f>
-        <v>2.4778701628723403</v>
+        <v>2.4150324329787236</v>
       </c>
       <c r="B6" s="60" t="s">
         <v>221</v>
@@ -16092,14 +16099,14 @@
       </c>
       <c r="I6" s="63">
         <f>N25</f>
-        <v>7.2021423231536374E-2</v>
+        <v>7.1610376967769854E-2</v>
       </c>
       <c r="J6" s="61" t="s">
         <v>224</v>
       </c>
       <c r="K6" s="69">
         <f>I5/G4</f>
-        <v>4915.2606037942123</v>
+        <v>5048.9649542865</v>
       </c>
       <c r="L6" s="70" t="s">
         <v>225</v>
@@ -16117,14 +16124,14 @@
     <row r="7" spans="1:16" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <f>O20/F12</f>
-        <v>17.493037574915508</v>
+        <v>17.049421607209915</v>
       </c>
       <c r="B7" s="72" t="s">
         <v>227</v>
       </c>
       <c r="C7" s="73">
         <f>F15/A3</f>
-        <v>6.343385275749322E-2</v>
+        <v>6.5084364465433475E-2</v>
       </c>
       <c r="D7" s="72" t="s">
         <v>228</v>
@@ -16151,7 +16158,7 @@
       </c>
       <c r="K7" s="79">
         <f>K6/K5-1</f>
-        <v>0.86060778037066799</v>
+        <v>0.92672551861922781</v>
       </c>
       <c r="L7" s="80" t="s">
         <v>231</v>
@@ -16464,7 +16471,7 @@
       </c>
       <c r="O14" s="106">
         <f>'[1]US Treasury Bonds'!$C$8</f>
-        <v>4.2709999999999998E-2</v>
+        <v>4.1210000000000004E-2</v>
       </c>
       <c r="P14" s="38"/>
     </row>
@@ -16509,7 +16516,7 @@
       </c>
       <c r="O15" s="107" cm="1">
         <f t="array" ref="O15">_FV(A1,"Beta")</f>
-        <v>0.68440000000000001</v>
+        <v>0.68459999999999999</v>
       </c>
       <c r="P15" s="38"/>
     </row>
@@ -16610,7 +16617,7 @@
       </c>
       <c r="O17" s="109">
         <f>(O14)+((O15)*(O16-O14))</f>
-        <v>7.0968876E-2</v>
+        <v>7.0504034000000007E-2</v>
       </c>
       <c r="P17" s="38"/>
     </row>
@@ -16686,22 +16693,22 @@
       </c>
       <c r="O20" s="110" cm="1">
         <f t="array" ref="O20">_FV(A1,"Market cap",TRUE)</f>
-        <v>46583959062</v>
+        <v>45402609740</v>
       </c>
       <c r="P20" s="38"/>
     </row>
     <row r="21" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="123" t="str" cm="1">
+      <c r="A21" s="124" t="str" cm="1">
         <f t="array" ref="A21">_FV(A1,"Industry")</f>
         <v>Specialty Retailers</v>
       </c>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="124" cm="1">
+      <c r="B21" s="124"/>
+      <c r="C21" s="124"/>
+      <c r="D21" s="125" cm="1">
         <f t="array" ref="D21">_FV(A1,"Year incorporated",TRUE)</f>
         <v>1991</v>
       </c>
-      <c r="E21" s="124"/>
+      <c r="E21" s="125"/>
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>
       <c r="H21" s="43"/>
@@ -16714,7 +16721,7 @@
       </c>
       <c r="O21" s="110">
         <f>O19+O20</f>
-        <v>49501005062</v>
+        <v>48319655740</v>
       </c>
       <c r="P21" s="38"/>
     </row>
@@ -16740,7 +16747,7 @@
       </c>
       <c r="O22" s="111">
         <f>(O19/O21)</f>
-        <v>5.8929025710617401E-2</v>
+        <v>6.0369759579748196E-2</v>
       </c>
       <c r="P22" s="38"/>
     </row>
@@ -16763,7 +16770,7 @@
       </c>
       <c r="O23" s="112">
         <f>O20/O21</f>
-        <v>0.94107097428938258</v>
+        <v>0.93963024042025178</v>
       </c>
       <c r="P23" s="38"/>
     </row>
@@ -16803,7 +16810,7 @@
       <c r="M25" s="43"/>
       <c r="N25" s="115">
         <f>(O22*O12)+(O23*O17)</f>
-        <v>7.2021423231536374E-2</v>
+        <v>7.1610376967769854E-2</v>
       </c>
       <c r="O25" s="116"/>
       <c r="P25" s="38"/>

</xml_diff>